<commit_message>
Updated Schematic, Pinout, and added labels to encoders in hubcode
</commit_message>
<xml_diff>
--- a/Docs/Pinout/Pinout.xlsx
+++ b/Docs/Pinout/Pinout.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\GitHub\Submarine-project\Docs\Pinout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\Submarine\Submarine-project\Docs\Pinout\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Arduino mega</t>
   </si>
@@ -131,13 +131,16 @@
     <t>RUNNING LIGHTS</t>
   </si>
   <si>
-    <t>6~8</t>
+    <t>SENS_PIN</t>
+  </si>
+  <si>
+    <t>6~7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -449,23 +452,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,12 +482,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -510,7 +513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -536,13 +539,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
       <c r="G5" t="s">
         <v>30</v>
       </c>
@@ -550,7 +559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -564,7 +573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -578,7 +587,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -592,7 +601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -603,10 +612,10 @@
         <v>34</v>
       </c>
       <c r="H9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
New STLs, Updated Pinout, Added Water sensors to schematic, minor IPT changes
</commit_message>
<xml_diff>
--- a/Docs/Pinout/Pinout.xlsx
+++ b/Docs/Pinout/Pinout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Arduino mega</t>
   </si>
@@ -71,12 +71,6 @@
     <t>0~2</t>
   </si>
   <si>
-    <t>39-41</t>
-  </si>
-  <si>
-    <t>WATER (PORTG 0~2)</t>
-  </si>
-  <si>
     <t>Encoder reader</t>
   </si>
   <si>
@@ -89,12 +83,6 @@
     <t>RELAY (PORTD 2~3)</t>
   </si>
   <si>
-    <t>WATER (PORTB 0~2)</t>
-  </si>
-  <si>
-    <t>13~15</t>
-  </si>
-  <si>
     <t>OUT-HIGH (PORTD 4~7)</t>
   </si>
   <si>
@@ -135,6 +123,9 @@
   </si>
   <si>
     <t>6~7</t>
+  </si>
+  <si>
+    <t>WATER_SENS_ANALOG</t>
   </si>
 </sst>
 </file>
@@ -453,15 +444,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
@@ -473,13 +464,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -495,19 +486,19 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
         <v>24</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -521,19 +512,19 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
         <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>29</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -547,13 +538,13 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -567,7 +558,7 @@
         <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H6">
         <v>3</v>
@@ -581,7 +572,7 @@
         <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H7">
         <v>4</v>
@@ -595,7 +586,7 @@
         <v>38</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H8">
         <v>5</v>
@@ -609,18 +600,10 @@
         <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Pressure Sensor to CAD and Schematic, updated gitignore
</commit_message>
<xml_diff>
--- a/Docs/Pinout/Pinout.xlsx
+++ b/Docs/Pinout/Pinout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Arduino mega</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>WATER_SENS_ANALOG</t>
+  </si>
+  <si>
+    <t>PRESSURE TRANSDUCER</t>
   </si>
 </sst>
 </file>
@@ -444,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,6 +609,14 @@
         <v>32</v>
       </c>
     </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>